<commit_message>
Excel Values Group Runner First Commit
First commit of excel value to run groups in testng
</commit_message>
<xml_diff>
--- a/TemplatePr2h/src/test/java/testData/Automation Test Cases.xlsx
+++ b/TemplatePr2h/src/test/java/testData/Automation Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prathamesh.lad@nanostuffs.com\FrameworkTemplate\Final-Maven-Framework\TemplatePr2h\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02166300-D827-4F9D-9832-5536C6BD1754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C9A1AA-D716-49AB-9896-B55DB278D0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3324" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -60,20 +60,35 @@
     <t>Chrome</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Title 1</t>
+  </si>
+  <si>
+    <t>Title 2</t>
+  </si>
+  <si>
+    <t>Title 4</t>
+  </si>
+  <si>
+    <t>Smoke</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,9 +114,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,7 +399,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,8 +435,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>45159</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -437,15 +451,15 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -460,15 +474,15 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>45158</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -483,15 +497,15 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
         <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -506,13 +520,14 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
         <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel to run testCases
Excel to run testcases with java main method
</commit_message>
<xml_diff>
--- a/TemplatePr2h/src/test/java/testData/Automation Test Cases.xlsx
+++ b/TemplatePr2h/src/test/java/testData/Automation Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prathamesh.lad@nanostuffs.com\FrameworkTemplate\Final-Maven-Framework\TemplatePr2h\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C9A1AA-D716-49AB-9896-B55DB278D0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3251614A-9696-47DE-9C16-10B90387FBE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="32">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -63,16 +63,64 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Title 1</t>
-  </si>
-  <si>
-    <t>Title 2</t>
-  </si>
-  <si>
-    <t>Title 4</t>
-  </si>
-  <si>
     <t>Smoke</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>TC_06</t>
+  </si>
+  <si>
+    <t>TC_07</t>
+  </si>
+  <si>
+    <t>TC_08</t>
+  </si>
+  <si>
+    <t>TC_09</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t>TC_11</t>
+  </si>
+  <si>
+    <t>TC_12</t>
+  </si>
+  <si>
+    <t>TC_13</t>
+  </si>
+  <si>
+    <t>TC_14</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Login with incorrect passoword</t>
+  </si>
+  <si>
+    <t>Homepage</t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Contact Us page</t>
   </si>
 </sst>
 </file>
@@ -396,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,10 +456,11 @@
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.44140625" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,11 +479,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -451,18 +500,21 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -474,18 +526,21 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -497,32 +552,298 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="G5" t="s">
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Excel yes no first commit
</commit_message>
<xml_diff>
--- a/TemplatePr2h/src/test/java/testData/Automation Test Cases.xlsx
+++ b/TemplatePr2h/src/test/java/testData/Automation Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prathamesh.lad@nanostuffs.com\FrameworkTemplate\Final-Maven-Framework\TemplatePr2h\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3251614A-9696-47DE-9C16-10B90387FBE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C267C8-E152-44E6-A050-D66799A98EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,7 +529,7 @@
         <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
@@ -630,10 +630,10 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H7" t="s">
         <v>11</v>
@@ -656,7 +656,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G8" t="s">
         <v>12</v>
@@ -682,7 +682,7 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G9" t="s">
         <v>12</v>
@@ -708,7 +708,7 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G10" t="s">
         <v>6</v>
@@ -734,7 +734,7 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G11" t="s">
         <v>12</v>
@@ -760,7 +760,7 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
@@ -786,7 +786,7 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G13" t="s">
         <v>12</v>
@@ -812,7 +812,7 @@
         <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G14" t="s">
         <v>6</v>
@@ -838,7 +838,7 @@
         <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
         <v>6</v>

</xml_diff>